<commit_message>
Correct image filenames in CROSSBOW
Signed-off-by: Richard Marston <rmarston@eonerc.rwth-aachen.de>
</commit_message>
<xml_diff>
--- a/excel-use-cases/CROSSBOW/HLU02-UC02/CROSSBOW-UHL02-UC2.xlsx
+++ b/excel-use-cases/CROSSBOW/HLU02-UC02/CROSSBOW-UHL02-UC2.xlsx
@@ -1410,7 +1410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="157">
   <si>
     <t xml:space="preserve">1 Description of the use case</t>
   </si>
@@ -1627,28 +1627,31 @@
     <t xml:space="preserve">Diagram URI value</t>
   </si>
   <si>
-    <t xml:space="preserve">HLU2-UC02-function.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLU2-UC02-component.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLU2-UC02-communication.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLU2-UC02-information.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLU2-UC02-canonical.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLU2-UC02-estandard.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLU2-UC02-activity.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLU2-UC02-sequence.png</t>
+    <t xml:space="preserve">HLU02-UC2-function.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLU02-UC2-COMPONENT.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLU02-UC2-COMMUNICATION.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLU02-UC2-INFORMATION.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLU02-UC2-CANONICAL.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLU02-UC2-STANDARD.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLU02-UC2-ACTIVITY.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLU02-UC2-FUNCTION.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLU02-UC2-SEQUENCE.png</t>
   </si>
   <si>
     <t xml:space="preserve">3 Technical details</t>
@@ -2328,22 +2331,24 @@
   </sheetPr>
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E34" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F34" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K40" activeCellId="0" sqref="K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1017" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1017" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2824,22 +2829,22 @@
         <v>75</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
       <c r="B43" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -2849,7 +2854,7 @@
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
       <c r="B44" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="12"/>
@@ -2859,7 +2864,7 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
       <c r="B45" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="12"/>
@@ -2869,55 +2874,55 @@
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
       <c r="B46" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H46" s="22" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
       <c r="B47" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G47" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
       <c r="B48" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="12"/>
@@ -2927,7 +2932,7 @@
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
       <c r="B49" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C49" s="24"/>
       <c r="D49" s="12"/>
@@ -2937,7 +2942,7 @@
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
       <c r="B50" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -2957,7 +2962,7 @@
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4"/>
       <c r="B52" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="12"/>
@@ -2967,7 +2972,7 @@
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
       <c r="B53" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="12"/>
@@ -2977,7 +2982,7 @@
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
       <c r="B54" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="12"/>
@@ -2987,7 +2992,7 @@
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
       <c r="B55" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="12"/>
@@ -2997,7 +3002,7 @@
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
       <c r="B56" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="12"/>
@@ -3007,7 +3012,7 @@
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
       <c r="B57" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="12"/>
@@ -3017,7 +3022,7 @@
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
       <c r="B58" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="12"/>
@@ -3031,17 +3036,17 @@
     </row>
     <row r="60" customFormat="false" ht="24.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4"/>
       <c r="B61" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
@@ -3051,7 +3056,7 @@
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4"/>
       <c r="B62" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C62" s="9" t="n">
         <v>1</v>
@@ -3065,13 +3070,13 @@
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4"/>
       <c r="B63" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
@@ -3079,7 +3084,7 @@
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4"/>
       <c r="B64" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C64" s="9"/>
       <c r="D64" s="12"/>
@@ -3089,13 +3094,13 @@
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4"/>
       <c r="B65" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
@@ -3103,13 +3108,13 @@
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4"/>
       <c r="B66" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E66" s="12"/>
       <c r="F66" s="12"/>
@@ -3117,10 +3122,10 @@
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4"/>
       <c r="B67" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
@@ -3128,10 +3133,10 @@
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4"/>
       <c r="B68" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E68" s="12"/>
       <c r="F68" s="12"/>
@@ -3139,7 +3144,7 @@
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4"/>
       <c r="B69" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
@@ -3149,22 +3154,22 @@
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4"/>
       <c r="B70" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H70" s="9"/>
       <c r="I70" s="9"/>
@@ -3173,7 +3178,7 @@
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4"/>
       <c r="B71" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C71" s="9" t="n">
         <v>1</v>
@@ -3197,22 +3202,22 @@
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="4"/>
       <c r="B72" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H72" s="9"/>
       <c r="I72" s="9"/>
@@ -3221,7 +3226,7 @@
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4"/>
       <c r="B73" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
@@ -3235,22 +3240,22 @@
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4"/>
       <c r="B74" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
@@ -3259,7 +3264,7 @@
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4"/>
       <c r="B75" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
@@ -3273,22 +3278,22 @@
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4"/>
       <c r="B76" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="9"/>
@@ -3297,22 +3302,22 @@
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4"/>
       <c r="B77" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F77" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C77" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>140</v>
-      </c>
       <c r="G77" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H77" s="9"/>
       <c r="I77" s="9"/>
@@ -3321,7 +3326,7 @@
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="18"/>
       <c r="B78" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C78" s="9" t="n">
         <v>1</v>
@@ -3343,7 +3348,7 @@
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="19"/>
       <c r="B79" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
@@ -3354,7 +3359,7 @@
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="6"/>
@@ -3364,7 +3369,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C81" s="9"/>
       <c r="D81" s="12"/>
@@ -3374,7 +3379,7 @@
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4"/>
       <c r="B82" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C82" s="9" t="n">
         <v>1</v>
@@ -3397,22 +3402,22 @@
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4"/>
       <c r="B83" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D83" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E83" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E83" s="12" t="s">
-        <v>149</v>
-      </c>
       <c r="F83" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H83" s="12"/>
       <c r="I83" s="12"/>
@@ -3420,22 +3425,22 @@
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4"/>
       <c r="B84" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F84" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="G84" s="27" t="s">
         <v>153</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="F84" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="G84" s="27" t="s">
-        <v>152</v>
       </c>
       <c r="H84" s="27"/>
       <c r="I84" s="27"/>
@@ -3463,19 +3468,19 @@
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="81.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="81.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add image metadata for OneNet/WECL-PT-*
Signed-off-by: Richard Marston <rmarston@eonerc.rwth-aachen.de>
</commit_message>
<xml_diff>
--- a/excel-use-cases/CROSSBOW/HLU02-UC02/CROSSBOW-UHL02-UC2.xlsx
+++ b/excel-use-cases/CROSSBOW/HLU02-UC02/CROSSBOW-UHL02-UC2.xlsx
@@ -1410,7 +1410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="156">
   <si>
     <t xml:space="preserve">1 Description of the use case</t>
   </si>
@@ -1627,7 +1627,7 @@
     <t xml:space="preserve">Diagram URI value</t>
   </si>
   <si>
-    <t xml:space="preserve">HLU02-UC2-function.png</t>
+    <t xml:space="preserve">HLU02-UC2-FUNCTION.png</t>
   </si>
   <si>
     <t xml:space="preserve">HLU02-UC2-COMPONENT.png</t>
@@ -1646,9 +1646,6 @@
   </si>
   <si>
     <t xml:space="preserve">HLU02-UC2-ACTIVITY.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLU02-UC2-FUNCTION.png</t>
   </si>
   <si>
     <t xml:space="preserve">HLU02-UC2-SEQUENCE.png</t>
@@ -2331,11 +2328,11 @@
   </sheetPr>
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F34" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K40" activeCellId="0" sqref="K40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C34" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.43"/>
@@ -2829,22 +2826,22 @@
         <v>75</v>
       </c>
       <c r="J41" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="K41" s="9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
       <c r="B43" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -2854,7 +2851,7 @@
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
       <c r="B44" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="12"/>
@@ -2864,7 +2861,7 @@
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
       <c r="B45" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="12"/>
@@ -2874,55 +2871,55 @@
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
       <c r="B46" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="D46" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="E46" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="F46" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="G46" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="G46" s="21" t="s">
+      <c r="H46" s="22" t="s">
         <v>87</v>
-      </c>
-      <c r="H46" s="22" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
       <c r="B47" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="D47" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="E47" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="F47" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="G47" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="H47" s="21" t="s">
         <v>94</v>
-      </c>
-      <c r="H47" s="21" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
       <c r="B48" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="12"/>
@@ -2932,7 +2929,7 @@
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
       <c r="B49" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C49" s="24"/>
       <c r="D49" s="12"/>
@@ -2942,7 +2939,7 @@
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
       <c r="B50" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -2962,7 +2959,7 @@
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4"/>
       <c r="B52" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="12"/>
@@ -2972,7 +2969,7 @@
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
       <c r="B53" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="12"/>
@@ -2982,7 +2979,7 @@
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
       <c r="B54" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="12"/>
@@ -2992,7 +2989,7 @@
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
       <c r="B55" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="12"/>
@@ -3002,7 +2999,7 @@
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
       <c r="B56" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="12"/>
@@ -3012,7 +3009,7 @@
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
       <c r="B57" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="12"/>
@@ -3022,7 +3019,7 @@
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
       <c r="B58" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="12"/>
@@ -3036,17 +3033,17 @@
     </row>
     <row r="60" customFormat="false" ht="24.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="C60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4"/>
       <c r="B61" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
@@ -3056,7 +3053,7 @@
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4"/>
       <c r="B62" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C62" s="9" t="n">
         <v>1</v>
@@ -3070,13 +3067,13 @@
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4"/>
       <c r="B63" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="D63" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
@@ -3084,7 +3081,7 @@
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4"/>
       <c r="B64" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C64" s="9"/>
       <c r="D64" s="12"/>
@@ -3094,13 +3091,13 @@
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4"/>
       <c r="B65" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" s="12" t="s">
         <v>113</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>114</v>
       </c>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
@@ -3108,13 +3105,13 @@
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4"/>
       <c r="B66" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="D66" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>117</v>
       </c>
       <c r="E66" s="12"/>
       <c r="F66" s="12"/>
@@ -3122,10 +3119,10 @@
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4"/>
       <c r="B67" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
@@ -3133,10 +3130,10 @@
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4"/>
       <c r="B68" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D68" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="E68" s="12"/>
       <c r="F68" s="12"/>
@@ -3144,7 +3141,7 @@
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4"/>
       <c r="B69" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
@@ -3154,22 +3151,22 @@
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4"/>
       <c r="B70" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F70" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C70" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>124</v>
-      </c>
       <c r="G70" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H70" s="9"/>
       <c r="I70" s="9"/>
@@ -3178,7 +3175,7 @@
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4"/>
       <c r="B71" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C71" s="9" t="n">
         <v>1</v>
@@ -3202,22 +3199,22 @@
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="4"/>
       <c r="B72" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="D72" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="E72" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="E72" s="9" t="s">
+      <c r="F72" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F72" s="9" t="s">
-        <v>130</v>
-      </c>
       <c r="G72" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H72" s="9"/>
       <c r="I72" s="9"/>
@@ -3226,7 +3223,7 @@
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4"/>
       <c r="B73" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
@@ -3240,22 +3237,22 @@
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4"/>
       <c r="B74" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C74" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="D74" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="E74" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="F74" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="9" t="s">
+      <c r="G74" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="G74" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
@@ -3264,7 +3261,7 @@
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4"/>
       <c r="B75" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
@@ -3278,22 +3275,22 @@
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4"/>
       <c r="B76" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="D76" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G76" s="9" t="s">
         <v>140</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="F76" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G76" s="9" t="s">
-        <v>141</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="9"/>
@@ -3302,22 +3299,22 @@
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4"/>
       <c r="B77" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C77" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D77" s="9" t="s">
+      <c r="F77" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E77" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>141</v>
-      </c>
       <c r="G77" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H77" s="9"/>
       <c r="I77" s="9"/>
@@ -3326,7 +3323,7 @@
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="18"/>
       <c r="B78" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C78" s="9" t="n">
         <v>1</v>
@@ -3348,7 +3345,7 @@
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="19"/>
       <c r="B79" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
@@ -3359,7 +3356,7 @@
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="6"/>
@@ -3369,7 +3366,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C81" s="9"/>
       <c r="D81" s="12"/>
@@ -3379,7 +3376,7 @@
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4"/>
       <c r="B82" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C82" s="9" t="n">
         <v>1</v>
@@ -3402,22 +3399,22 @@
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4"/>
       <c r="B83" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="D83" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="D83" s="12" t="s">
+      <c r="E83" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F83" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="E83" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="F83" s="12" t="s">
+      <c r="G83" s="12" t="s">
         <v>152</v>
-      </c>
-      <c r="G83" s="12" t="s">
-        <v>153</v>
       </c>
       <c r="H83" s="12"/>
       <c r="I83" s="12"/>
@@ -3425,22 +3422,22 @@
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4"/>
       <c r="B84" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C84" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D84" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="D84" s="12" t="s">
+      <c r="E84" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F84" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="E84" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="F84" s="27" t="s">
+      <c r="G84" s="27" t="s">
         <v>152</v>
-      </c>
-      <c r="G84" s="27" t="s">
-        <v>153</v>
       </c>
       <c r="H84" s="27"/>
       <c r="I84" s="27"/>
@@ -3468,19 +3465,19 @@
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="81.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>